<commit_message>
retrait style dans html
</commit_message>
<xml_diff>
--- a/seo.xlsx
+++ b/seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
@@ -76,28 +76,115 @@
     <t xml:space="preserve">couleur texte pas assez visible</t>
   </si>
   <si>
+    <t xml:space="preserve">changer la taille du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on ne voit pas bien ce qu’il y a écrit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">« accueil » non visible sur « contact »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un margin-right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on ne voit pas le mot accueil en entier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trop d’annuaires </t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever des annuaires </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a trop d’annuaires sur la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un minimum d’annuaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formulaire à refaire sur « contact »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agrandir le formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le formulaire n’est pas assez lisible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agrandir les formulaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">« page2 » sur page contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever « page2 »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on revient sur la même page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirer « page2 »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">point sur liste contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever les points de décoration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un list-style-decoration:none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">texte caché</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on ne voit pas le texte</t>
+  </si>
+  <si>
     <t xml:space="preserve">changer la couleur du texte</t>
   </si>
   <si>
-    <t xml:space="preserve">on ne voit pas bien ce qu’il y a écrit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">avis personnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">« accueil » non visible sur « contact »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trop d’annuaires </t>
-  </si>
-  <si>
-    <t xml:space="preserve">formulaire à refaire sur « contact »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indentation des h2 et h3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">balise title page2 « contact »</t>
+    <t xml:space="preserve">Accueil sur index html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever Accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on s’y trouve déjà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le point sur H1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever le point à la fin du titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever le point </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste 1 et 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever liste 1 et 2 sur annuaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on n’en a pas besoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirer liste 1 et 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur icône réseaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur des icônes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cela ne se voit pas très bien en blanc</t>
   </si>
 </sst>
 </file>
@@ -295,17 +382,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21"/>
@@ -405,39 +492,143 @@
         <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
mise en page de contact
</commit_message>
<xml_diff>
--- a/seo.xlsx
+++ b/seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
@@ -176,15 +176,6 @@
   </si>
   <si>
     <t xml:space="preserve">retirer liste 1 et 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">couleur icône réseaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">changer la couleur des icônes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cela ne se voit pas très bien en blanc</t>
   </si>
 </sst>
 </file>
@@ -384,11 +375,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.52"/>
@@ -615,20 +606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
changement de noms des photos
</commit_message>
<xml_diff>
--- a/seo.xlsx
+++ b/seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
@@ -82,13 +82,16 @@
     <t xml:space="preserve">on ne voit pas bien ce qu’il y a écrit </t>
   </si>
   <si>
-    <t xml:space="preserve">« accueil » non visible sur « contact »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre un margin-right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on ne voit pas le mot accueil en entier</t>
+    <t xml:space="preserve">Liste 1 et 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever liste 1 et 2 sur annuaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ça ne sert à rien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirer liste 1 et 2</t>
   </si>
   <si>
     <t xml:space="preserve">trop d’annuaires </t>
@@ -127,13 +130,16 @@
     <t xml:space="preserve">retirer « page2 »</t>
   </si>
   <si>
-    <t xml:space="preserve">point sur liste contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enlever les points de décoration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre un list-style-decoration:none</t>
+    <t xml:space="preserve">le point sur H1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever le point à la fin du titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il n’y a pas besoin de point à la fin du titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enlever le point </t>
   </si>
   <si>
     <t xml:space="preserve">texte caché</t>
@@ -157,25 +163,52 @@
     <t xml:space="preserve">on s’y trouve déjà</t>
   </si>
   <si>
-    <t xml:space="preserve">le point sur H1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enlever le point à la fin du titre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enlever le point </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste 1 et 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enlever liste 1 et 2 sur annuaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on n’en a pas besoin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retirer liste 1 et 2</t>
+    <t xml:space="preserve">images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer le nom des images en jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cela prend trop de temps pour le navigateur de les télécharger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renommer les images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">et-line.min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirer .min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">le et-line.min n’existe pas les modifications ne s’appliquent pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirer .min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap.min sur contact.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le bootstrap.min n’existe pas les modifications ne s’appliquent pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font-awesome.min sur contact.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le font-awesome n’existe pas les modifications ne s’appliquent pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur liste annuaires et partenaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur des liens sur les listes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on ne voit pas la différence entre les titres et les liens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur </t>
   </si>
 </sst>
 </file>
@@ -376,15 +409,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
@@ -497,118 +530,163 @@
         <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>